<commit_message>
Fix 2 sites, add 3 cars
</commit_message>
<xml_diff>
--- a/xlsx/tumen.xlsx
+++ b/xlsx/tumen.xlsx
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>2084990</v>
+        <v>2122990</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -4785,7 +4785,7 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>2198990</v>
+        <v>2236990</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
@@ -4925,6 +4925,14 @@
           <t>https://autotumen.ru/cars/geely/cityray/</t>
         </is>
       </c>
+      <c r="H89" t="n">
+        <v>2399990</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>https://bazis-motors.ru/cars/geely/cityray/</t>
+        </is>
+      </c>
       <c r="J89" t="n">
         <v>1579000</v>
       </c>
@@ -5609,14 +5617,6 @@
           <t>https://china-avto-tumen.ru/katalog-avtomobiley163538/geely/tugella/geely-tugella-2/</t>
         </is>
       </c>
-      <c r="H103" t="n">
-        <v>3395990</v>
-      </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>https://bazis-motors.ru/cars/geely/tugella/</t>
-        </is>
-      </c>
       <c r="J103" t="n">
         <v>2249990</v>
       </c>
@@ -7985,6 +7985,16 @@
       <c r="E155" t="inlineStr">
         <is>
           <t>https://autotumen.ru/cars/jaecoo/j8/</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>3079000</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>https://autocentr-72.ru/auto/jaecoo/j8/</t>
         </is>
       </c>
       <c r="J155" t="n">

</xml_diff>